<commit_message>
support for wekwikgene https://github.com/manulera/OpenCloning_backend/issues/263
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -20,33 +20,34 @@
     <sheet name="UploadedFileSource" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="RepositoryIdSource" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="AddGeneIdSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="BenchlingUrlSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="SnapGenePlasmidSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="EuroscarfSource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="IGEMSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="SequenceCutSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="SimpleSequenceLocation" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="AssemblyFragment" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="AssemblySource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="PCRSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="LigationSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="HomologousRecombinationSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="GibsonAssemblySource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="InFusionSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="GatewaySource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="CRISPRSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="OligoHybridizationSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="CloningStrategy" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="AnnotationReport" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="AnnotationSource" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="AssociatedFile" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="SequencingFile" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="WekWikGeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="BenchlingUrlSource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="SnapGenePlasmidSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="EuroscarfSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="IGEMSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SequenceCutSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="SimpleSequenceLocation" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="AssemblyFragment" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="AssemblySource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="PCRSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="LigationSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="HomologousRecombinationSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="GibsonAssemblySource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="InFusionSource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="GatewaySource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="CRISPRSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="OligoHybridizationSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="CloningStrategy" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="AnnotationReport" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="AnnotationSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="AssociatedFile" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="SequencingFile" sheetId="41" state="visible" r:id="rId41"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -750,6 +751,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -805,7 +872,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -866,7 +933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -927,7 +994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -993,7 +1060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1074,7 +1141,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>primer_design</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1130,7 +1238,99 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1147,53 +1347,53 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>reverse_complemented</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>circular</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>primer_design</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
+          <t>assembly</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1227,246 +1427,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>left_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>right_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>reverse_complemented</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1763,6 +1774,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1818,7 +1885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1889,7 +1956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1950,7 +2017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2011,7 +2078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2057,7 +2124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2103,7 +2170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2129,7 +2196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2225,7 +2292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2291,7 +2358,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2337,48 +2445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
support for SEVA plasmids https://github.com/manulera/OpenCloning_backend/issues/268
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -21,34 +21,35 @@
     <sheet name="RepositoryIdSource" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="AddGeneIdSource" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="WekWikGeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="BenchlingUrlSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SnapGenePlasmidSource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="EuroscarfSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="IGEMSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="SequenceCutSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="SimpleSequenceLocation" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="AssemblyFragment" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="AssemblySource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="PCRSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="LigationSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="HomologousRecombinationSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="GibsonAssemblySource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="InFusionSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="GatewaySource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="CRISPRSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="OligoHybridizationSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="CloningStrategy" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="AnnotationReport" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="AnnotationSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="ReverseComplementSource" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AssociatedFile" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="SequencingFile" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SEVASource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="BenchlingUrlSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SnapGenePlasmidSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="EuroscarfSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="IGEMSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SequenceCutSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SimpleSequenceLocation" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="AssemblyFragment" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="AssemblySource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PCRSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="LigationSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="HomologousRecombinationSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="GibsonAssemblySource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="InFusionSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="GatewaySource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="CRISPRSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="OligoHybridizationSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CloningStrategy" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="AnnotationReport" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="AnnotationSource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="ReverseComplementSource" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AssociatedFile" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SequencingFile" sheetId="43" state="visible" r:id="rId43"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -665,7 +666,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -739,7 +740,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -805,7 +806,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -818,6 +819,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -866,14 +933,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -927,14 +994,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -988,14 +1055,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1054,14 +1121,55 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>primer_design</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1142,7 +1250,155 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1159,53 +1415,53 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>reverse_complemented</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>circular</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>primer_design</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
+          <t>assembly</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1239,302 +1495,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>left_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>right_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>reverse_complemented</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1831,6 +1842,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1886,7 +1953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1957,7 +2024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2018,7 +2085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2079,7 +2146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2125,7 +2192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2171,7 +2238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2197,7 +2264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2293,7 +2360,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2359,48 +2467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2446,7 +2513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2492,7 +2559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
support for SEVA plasmids https://github.com/manulera/OpenCloning_backend/issues/268 (#34)
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -21,34 +21,35 @@
     <sheet name="RepositoryIdSource" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="AddGeneIdSource" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="WekWikGeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="BenchlingUrlSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="SnapGenePlasmidSource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="EuroscarfSource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="IGEMSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="SequenceCutSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="SimpleSequenceLocation" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="AssemblyFragment" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="AssemblySource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="PCRSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="LigationSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="HomologousRecombinationSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="GibsonAssemblySource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="InFusionSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="GatewaySource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="CRISPRSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="OligoHybridizationSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="CloningStrategy" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="AnnotationReport" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="AnnotationSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="ReverseComplementSource" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AssociatedFile" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="SequencingFile" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SEVASource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="BenchlingUrlSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="SnapGenePlasmidSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="EuroscarfSource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="IGEMSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="SequenceCutSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SimpleSequenceLocation" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="AssemblyFragment" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="AssemblySource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PCRSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="LigationSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="HomologousRecombinationSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="GibsonAssemblySource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="InFusionSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="GatewaySource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="CRISPRSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="OligoHybridizationSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CloningStrategy" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="AnnotationReport" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="AnnotationSource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="ReverseComplementSource" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AssociatedFile" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="SequencingFile" sheetId="43" state="visible" r:id="rId43"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -665,7 +666,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -739,7 +740,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -805,7 +806,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -818,6 +819,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -866,14 +933,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -927,14 +994,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -988,14 +1055,14 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1054,14 +1121,55 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>primer_design</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1142,7 +1250,155 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>left_edge</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>right_edge</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1159,53 +1415,53 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>reverse_complemented</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>circular</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>primer_design</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
+          <t>assembly</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -1239,302 +1495,57 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>left_edge</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>right_edge</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>left_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>right_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>reverse_complemented</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1831,6 +1842,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1886,7 +1953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1957,7 +2024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2018,7 +2085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2079,7 +2146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2125,7 +2192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2171,7 +2238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2197,7 +2264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2293,7 +2360,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2359,48 +2467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2446,7 +2513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2492,7 +2559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>